<commit_message>
commit for driver and shift classes
</commit_message>
<xml_diff>
--- a/Input Data/roaster_v2.xlsx
+++ b/Input Data/roaster_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jp/Library/Mobile Documents/com~apple~CloudDocs/testMVP/CDEV3300-Gate-Gourmet-Scheduling/Parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A306A6DB-546C-8C4B-97A4-E90BBC051ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF6246C-754C-0443-AF5A-B8A316B38D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{49BF6443-8E52-F24C-98C3-C460BC63957C}"/>
   </bookViews>
@@ -210,10 +210,17 @@
   <numFmts count="1">
     <numFmt numFmtId="168" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -225,18 +232,12 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -277,15 +278,15 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,7 +636,7 @@
   <dimension ref="A1:Y56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="30" customHeight="1"/>
@@ -716,7 +717,7 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="3"/>
       <c r="F2" s="4"/>
@@ -902,7 +903,7 @@
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="5"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -933,7 +934,7 @@
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -964,7 +965,7 @@
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -995,7 +996,7 @@
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1026,7 +1027,7 @@
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1057,7 +1058,7 @@
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1088,7 +1089,7 @@
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1119,7 +1120,7 @@
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1150,7 +1151,7 @@
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1181,7 +1182,7 @@
       <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="3"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1212,7 +1213,7 @@
       <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1243,7 +1244,7 @@
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="3"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1274,7 +1275,7 @@
       <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="3"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1305,7 +1306,7 @@
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -1336,7 +1337,7 @@
       <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="3"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1367,7 +1368,7 @@
       <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="C23" s="3"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1398,7 +1399,7 @@
       <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="1"/>
+      <c r="C24" s="3"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1429,7 +1430,7 @@
       <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="1"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1460,7 +1461,7 @@
       <c r="B26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="1"/>
+      <c r="C26" s="3"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -1491,7 +1492,7 @@
       <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="1"/>
+      <c r="C27" s="3"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1522,7 +1523,7 @@
       <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" s="3"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1553,7 +1554,7 @@
       <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="1"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1584,7 +1585,7 @@
       <c r="B30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1615,7 +1616,7 @@
       <c r="B31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="1"/>
+      <c r="C31" s="3"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -1646,7 +1647,7 @@
       <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="1"/>
+      <c r="C32" s="3"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1677,7 +1678,7 @@
       <c r="B33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="1"/>
+      <c r="C33" s="3"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -1708,7 +1709,7 @@
       <c r="B34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="1"/>
+      <c r="C34" s="3"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -1739,7 +1740,7 @@
       <c r="B35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="1"/>
+      <c r="C35" s="3"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -1770,7 +1771,7 @@
       <c r="B36" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="1"/>
+      <c r="C36" s="3"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -1801,7 +1802,7 @@
       <c r="B37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="1"/>
+      <c r="C37" s="3"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -1832,7 +1833,7 @@
       <c r="B38" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="1"/>
+      <c r="C38" s="3"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -1863,7 +1864,7 @@
       <c r="B39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="1"/>
+      <c r="C39" s="3"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -1894,7 +1895,7 @@
       <c r="B40" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="1"/>
+      <c r="C40" s="3"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -1925,7 +1926,7 @@
       <c r="B41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="1"/>
+      <c r="C41" s="3"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -1956,7 +1957,7 @@
       <c r="B42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="1"/>
+      <c r="C42" s="3"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -1987,7 +1988,7 @@
       <c r="B43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="1"/>
+      <c r="C43" s="3"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -2018,7 +2019,7 @@
       <c r="B44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="1"/>
+      <c r="C44" s="3"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -2049,7 +2050,7 @@
       <c r="B45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="1"/>
+      <c r="C45" s="3"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -2080,7 +2081,7 @@
       <c r="B46" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="1"/>
+      <c r="C46" s="3"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -2111,7 +2112,7 @@
       <c r="B47" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="1"/>
+      <c r="C47" s="3"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -2142,7 +2143,7 @@
       <c r="B48" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="1"/>
+      <c r="C48" s="3"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2173,7 +2174,7 @@
       <c r="B49" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="1"/>
+      <c r="C49" s="3"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -2204,7 +2205,7 @@
       <c r="B50" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="1"/>
+      <c r="C50" s="3"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -2235,7 +2236,7 @@
       <c r="B51" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="1"/>
+      <c r="C51" s="3"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -2266,7 +2267,7 @@
       <c r="B52" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C52" s="1"/>
+      <c r="C52" s="3"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -2297,7 +2298,7 @@
       <c r="B53" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C53" s="1"/>
+      <c r="C53" s="3"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -2328,7 +2329,7 @@
       <c r="B54" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C54" s="1"/>
+      <c r="C54" s="3"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -2359,7 +2360,7 @@
       <c r="B55" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C55" s="1"/>
+      <c r="C55" s="3"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -2390,7 +2391,7 @@
       <c r="B56" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C56" s="1"/>
+      <c r="C56" s="3"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>

</xml_diff>